<commit_message>
Updates on 7/24/23 with YBP1 CenDiaLg E-2 count of 1 added and re-run
</commit_message>
<xml_diff>
--- a/Notes/Presence_Evidence Table.xlsx
+++ b/Notes/Presence_Evidence Table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/allisonadams/My files/Thesis/Microplankton/MicroplanktonAnalysis/Notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EC10F2D-C682-7744-AC65-943F3868EF28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13B07E1-D276-0A47-848E-727B2253FFB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24600" windowHeight="15500" activeTab="1" xr2:uid="{37D73330-5E25-A441-8FFC-4BED75A08336}"/>
   </bookViews>
@@ -16,18 +16,21 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet1 (2)" sheetId="3" r:id="rId2"/>
     <sheet name="By IRbio" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="By Evidence" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'By Evidence'!$B$1:$G$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">'By IRbio'!$B$1:$G$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$F$93</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="1">'Sheet1 (2)'!$A$1:$F$93</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="3">Sheet2!$A$1:$C$22</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">Sheet2!$A$1:$C$22</definedName>
+    <definedName name="_xlnm.Print_Titles" localSheetId="3">'By Evidence'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">'By IRbio'!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">Sheet1!$1:$1</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'Sheet1 (2)'!$1:$1</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,8 +50,26 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={AE5138C8-B870-6948-A1F2-3E2568870E9F}</author>
+  </authors>
+  <commentList>
+    <comment ref="D1" authorId="0" shapeId="0" xr:uid="{AE5138C8-B870-6948-A1F2-3E2568870E9F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Hello</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1319" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1794" uniqueCount="78">
   <si>
     <t>Event</t>
   </si>
@@ -288,7 +309,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -380,6 +401,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="12">
@@ -815,7 +842,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -990,6 +1017,24 @@
     <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
@@ -999,33 +1044,21 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="19" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="58">
+  <dxfs count="69">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1043,6 +1076,87 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1FE7F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7DCFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB8B0EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1108,6 +1222,26 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -1128,11 +1262,222 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF9C5700"/>
       </font>
       <fill>
         <patternFill>
           <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1FE7F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7DCFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB8B0EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="5" tint="-0.499984740745262"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1177,12 +1522,33 @@
       </fill>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF1FE7F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFB8B0EE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFF7DCFC"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <font>
-        <color rgb="FF9C0006"/>
+        <color theme="4" tint="-0.24994659260841701"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
+          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1218,132 +1584,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB8B0EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF1FE7F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7DCFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1390,6 +1635,13 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor rgb="FF1FE7F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor rgb="FFB8B0EE"/>
         </patternFill>
       </fill>
@@ -1397,44 +1649,7 @@
     <dxf>
       <fill>
         <patternFill>
-          <bgColor rgb="FF1FE7F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
           <bgColor rgb="FFF7DCFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="5" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1460,11 +1675,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1480,92 +1695,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFB8B0EE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF1FE7F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFF7DCFC"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color theme="5" tint="-0.499984740745262"/>
       </font>
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1598,6 +1732,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Allison Adams" id="{B95CC702-0B4B-B947-ACC3-EF2E4BED24DF}" userId="S::aadams5@mail.sfsu.edu::32253c16-4a89-408b-906a-6e3154c8643b" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1895,6 +2035,14 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="D1" dT="2023-07-15T21:19:38.55" personId="{B95CC702-0B4B-B947-ACC3-EF2E4BED24DF}" id="{AE5138C8-B870-6948-A1F2-3E2568870E9F}">
+    <text>Hello</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F594588A-9BB6-9E46-A541-9A689C6B603B}">
   <dimension ref="A1:F93"/>
@@ -1928,7 +2076,7 @@
       </c>
     </row>
     <row r="2" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="45" t="s">
@@ -1948,7 +2096,7 @@
       </c>
     </row>
     <row r="3" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="48" t="s">
         <v>6</v>
       </c>
@@ -1966,7 +2114,7 @@
       </c>
     </row>
     <row r="4" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="45" t="s">
         <v>7</v>
       </c>
@@ -1984,7 +2132,7 @@
       </c>
     </row>
     <row r="5" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="48" t="s">
         <v>8</v>
       </c>
@@ -2002,7 +2150,7 @@
       </c>
     </row>
     <row r="6" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
@@ -2020,7 +2168,7 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="51" t="s">
         <v>10</v>
       </c>
@@ -2038,7 +2186,7 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="45" t="s">
@@ -2058,7 +2206,7 @@
       </c>
     </row>
     <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="48" t="s">
         <v>6</v>
       </c>
@@ -2076,7 +2224,7 @@
       </c>
     </row>
     <row r="10" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="45" t="s">
         <v>7</v>
       </c>
@@ -2094,7 +2242,7 @@
       </c>
     </row>
     <row r="11" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
@@ -2110,7 +2258,7 @@
       </c>
     </row>
     <row r="12" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="45" t="s">
         <v>9</v>
       </c>
@@ -2128,7 +2276,7 @@
       </c>
     </row>
     <row r="13" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="51" t="s">
         <v>10</v>
       </c>
@@ -2146,7 +2294,7 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="72" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="45" t="s">
@@ -2166,7 +2314,7 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="48" t="s">
         <v>6</v>
       </c>
@@ -2184,7 +2332,7 @@
       </c>
     </row>
     <row r="16" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="45" t="s">
         <v>7</v>
       </c>
@@ -2202,7 +2350,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="48" t="s">
         <v>8</v>
       </c>
@@ -2220,7 +2368,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="45" t="s">
         <v>9</v>
       </c>
@@ -2238,7 +2386,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="51" t="s">
         <v>10</v>
       </c>
@@ -2256,7 +2404,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="72" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="45" t="s">
@@ -2276,7 +2424,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="48" t="s">
         <v>6</v>
       </c>
@@ -2294,7 +2442,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="45" t="s">
         <v>7</v>
       </c>
@@ -2312,7 +2460,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="48" t="s">
         <v>8</v>
       </c>
@@ -2330,7 +2478,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="45" t="s">
         <v>9</v>
       </c>
@@ -2348,7 +2496,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="51" t="s">
         <v>10</v>
       </c>
@@ -2366,7 +2514,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="72" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="48" t="s">
@@ -2386,7 +2534,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="45" t="s">
         <v>6</v>
       </c>
@@ -2404,7 +2552,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="48" t="s">
         <v>7</v>
       </c>
@@ -2422,7 +2570,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="45" t="s">
         <v>8</v>
       </c>
@@ -2438,7 +2586,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="48" t="s">
         <v>9</v>
       </c>
@@ -2456,7 +2604,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="62" t="s">
         <v>10</v>
       </c>
@@ -2474,7 +2622,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="72" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="48" t="s">
@@ -2494,7 +2642,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="45" t="s">
         <v>6</v>
       </c>
@@ -2512,7 +2660,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65"/>
+      <c r="A34" s="73"/>
       <c r="B34" s="48" t="s">
         <v>7</v>
       </c>
@@ -2530,7 +2678,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="45" t="s">
         <v>8</v>
       </c>
@@ -2548,7 +2696,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
+      <c r="A36" s="73"/>
       <c r="B36" s="48" t="s">
         <v>9</v>
       </c>
@@ -2566,7 +2714,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="62" t="s">
         <v>10</v>
       </c>
@@ -2584,7 +2732,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="72" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="48" t="s">
@@ -2604,7 +2752,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="65"/>
+      <c r="A39" s="73"/>
       <c r="B39" s="45" t="s">
         <v>6</v>
       </c>
@@ -2620,7 +2768,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="65"/>
+      <c r="A40" s="73"/>
       <c r="B40" s="48" t="s">
         <v>7</v>
       </c>
@@ -2638,7 +2786,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="65"/>
+      <c r="A41" s="73"/>
       <c r="B41" s="45" t="s">
         <v>8</v>
       </c>
@@ -2654,7 +2802,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65"/>
+      <c r="A42" s="73"/>
       <c r="B42" s="48" t="s">
         <v>9</v>
       </c>
@@ -2672,7 +2820,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="62" t="s">
         <v>10</v>
       </c>
@@ -2690,7 +2838,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="72" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="45" t="s">
@@ -2708,7 +2856,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
+      <c r="A45" s="73"/>
       <c r="B45" s="48" t="s">
         <v>6</v>
       </c>
@@ -2724,7 +2872,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
+      <c r="A46" s="73"/>
       <c r="B46" s="45" t="s">
         <v>7</v>
       </c>
@@ -2742,7 +2890,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="65"/>
+      <c r="A47" s="73"/>
       <c r="B47" s="48" t="s">
         <v>8</v>
       </c>
@@ -2758,7 +2906,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
+      <c r="A48" s="73"/>
       <c r="B48" s="45" t="s">
         <v>9</v>
       </c>
@@ -2776,7 +2924,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="66"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="51" t="s">
         <v>10</v>
       </c>
@@ -2794,7 +2942,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="72" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="48" t="s">
@@ -2812,7 +2960,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
+      <c r="A51" s="73"/>
       <c r="B51" s="45" t="s">
         <v>6</v>
       </c>
@@ -2828,7 +2976,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
+      <c r="A52" s="73"/>
       <c r="B52" s="48" t="s">
         <v>7</v>
       </c>
@@ -2844,7 +2992,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="65"/>
+      <c r="A53" s="73"/>
       <c r="B53" s="45" t="s">
         <v>8</v>
       </c>
@@ -2860,7 +3008,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
+      <c r="A54" s="73"/>
       <c r="B54" s="48" t="s">
         <v>9</v>
       </c>
@@ -2878,7 +3026,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="66"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="62" t="s">
         <v>10</v>
       </c>
@@ -2896,7 +3044,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="72" t="s">
         <v>57</v>
       </c>
       <c r="B56" s="48" t="s">
@@ -2914,7 +3062,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
+      <c r="A57" s="73"/>
       <c r="B57" s="45" t="s">
         <v>6</v>
       </c>
@@ -2930,7 +3078,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
+      <c r="A58" s="73"/>
       <c r="B58" s="48" t="s">
         <v>7</v>
       </c>
@@ -2946,7 +3094,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="73"/>
       <c r="B59" s="45" t="s">
         <v>8</v>
       </c>
@@ -2962,7 +3110,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="73"/>
       <c r="B60" s="48" t="s">
         <v>9</v>
       </c>
@@ -2980,7 +3128,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="62" t="s">
         <v>10</v>
       </c>
@@ -2998,7 +3146,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="64" t="s">
+      <c r="A62" s="72" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="59" t="s">
@@ -3016,7 +3164,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="73"/>
       <c r="B63" s="45" t="s">
         <v>6</v>
       </c>
@@ -3032,7 +3180,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="73"/>
       <c r="B64" s="48" t="s">
         <v>7</v>
       </c>
@@ -3050,7 +3198,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="73"/>
       <c r="B65" s="45" t="s">
         <v>8</v>
       </c>
@@ -3066,7 +3214,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
+      <c r="A66" s="73"/>
       <c r="B66" s="48" t="s">
         <v>9</v>
       </c>
@@ -3082,7 +3230,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="66"/>
+      <c r="A67" s="74"/>
       <c r="B67" s="62" t="s">
         <v>10</v>
       </c>
@@ -3098,7 +3246,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="64" t="s">
+      <c r="A68" s="72" t="s">
         <v>18</v>
       </c>
       <c r="B68" s="48" t="s">
@@ -3116,7 +3264,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="73"/>
       <c r="B69" s="45" t="s">
         <v>6</v>
       </c>
@@ -3132,7 +3280,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="73"/>
       <c r="B70" s="48" t="s">
         <v>7</v>
       </c>
@@ -3148,7 +3296,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="73"/>
       <c r="B71" s="45" t="s">
         <v>8</v>
       </c>
@@ -3164,7 +3312,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="73"/>
       <c r="B72" s="48" t="s">
         <v>9</v>
       </c>
@@ -3180,7 +3328,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="66"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="62" t="s">
         <v>10</v>
       </c>
@@ -3198,7 +3346,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B74" s="45" t="s">
@@ -3216,7 +3364,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
+      <c r="A75" s="73"/>
       <c r="B75" s="48" t="s">
         <v>6</v>
       </c>
@@ -3232,7 +3380,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="73"/>
       <c r="B76" s="45" t="s">
         <v>7</v>
       </c>
@@ -3248,7 +3396,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="73"/>
       <c r="B77" s="48" t="s">
         <v>8</v>
       </c>
@@ -3264,7 +3412,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="73"/>
       <c r="B78" s="45" t="s">
         <v>9</v>
       </c>
@@ -3280,7 +3428,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
+      <c r="A79" s="74"/>
       <c r="B79" s="51" t="s">
         <v>10</v>
       </c>
@@ -3298,7 +3446,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="64" t="s">
+      <c r="A80" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B80" s="45" t="s">
@@ -3316,7 +3464,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="65"/>
+      <c r="A81" s="73"/>
       <c r="B81" s="48" t="s">
         <v>6</v>
       </c>
@@ -3332,7 +3480,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
+      <c r="A82" s="73"/>
       <c r="B82" s="45" t="s">
         <v>7</v>
       </c>
@@ -3348,7 +3496,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="65"/>
+      <c r="A83" s="73"/>
       <c r="B83" s="48" t="s">
         <v>8</v>
       </c>
@@ -3364,7 +3512,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="65"/>
+      <c r="A84" s="73"/>
       <c r="B84" s="45" t="s">
         <v>9</v>
       </c>
@@ -3380,7 +3528,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
+      <c r="A85" s="74"/>
       <c r="B85" s="51" t="s">
         <v>10</v>
       </c>
@@ -3444,36 +3592,36 @@
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <conditionalFormatting sqref="A3:A7">
-    <cfRule type="containsText" dxfId="57" priority="10" stopIfTrue="1" operator="containsText" text="LH">
+    <cfRule type="containsText" dxfId="68" priority="10" stopIfTrue="1" operator="containsText" text="LH">
       <formula>NOT(ISERROR(SEARCH("LH",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C85">
-    <cfRule type="containsText" dxfId="56" priority="9" operator="containsText" text="LH">
+    <cfRule type="containsText" dxfId="67" priority="12" operator="containsText" text="HH">
+      <formula>NOT(ISERROR(SEARCH("HH",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="66" priority="15" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="65" priority="13" operator="containsText" text="&lt;100">
+      <formula>NOT(ISERROR(SEARCH("&lt;100",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="64" priority="9" operator="containsText" text="LH">
       <formula>NOT(ISERROR(SEARCH("LH",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="63" priority="11" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="54" priority="12" operator="containsText" text="HH">
-      <formula>NOT(ISERROR(SEARCH("HH",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="53" priority="13" operator="containsText" text="&lt;100">
-      <formula>NOT(ISERROR(SEARCH("&lt;100",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="52" priority="15" operator="containsText" text="T">
-      <formula>NOT(ISERROR(SEARCH("T",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D85">
-    <cfRule type="endsWith" dxfId="51" priority="1" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="62" priority="1" operator="endsWith" text="*">
       <formula>RIGHT(D2,LEN("*"))="*"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="50" priority="3" operator="endsWith" text="~">
+    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="P+">
+      <formula>NOT(ISERROR(SEARCH("P+",D2)))</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="60" priority="3" operator="endsWith" text="~">
       <formula>RIGHT(D2,LEN("~"))="~"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="P+">
-      <formula>NOT(ISERROR(SEARCH("P+",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F85">
@@ -3487,7 +3635,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="47" priority="228" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="58" priority="228" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3538,11 +3686,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65CEAE2-D04F-3244-B03A-F177DF32416F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C65CEAE2-D04F-3244-B03A-F177DF32416F}">
   <dimension ref="A1:V93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3569,7 +3717,7 @@
       </c>
     </row>
     <row r="2" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="67" t="s">
+      <c r="A2" s="70" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="45" t="s">
@@ -3589,7 +3737,7 @@
       </c>
     </row>
     <row r="3" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="67"/>
+      <c r="A3" s="70"/>
       <c r="B3" s="48" t="s">
         <v>6</v>
       </c>
@@ -3607,7 +3755,7 @@
       </c>
     </row>
     <row r="4" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="67"/>
+      <c r="A4" s="70"/>
       <c r="B4" s="45" t="s">
         <v>7</v>
       </c>
@@ -3625,7 +3773,7 @@
       </c>
     </row>
     <row r="5" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="70"/>
       <c r="B5" s="48" t="s">
         <v>8</v>
       </c>
@@ -3643,7 +3791,7 @@
       </c>
     </row>
     <row r="6" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="70"/>
       <c r="B6" s="45" t="s">
         <v>9</v>
       </c>
@@ -3661,7 +3809,7 @@
       </c>
     </row>
     <row r="7" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="68"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="51" t="s">
         <v>10</v>
       </c>
@@ -3682,7 +3830,7 @@
       </c>
     </row>
     <row r="8" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="72" t="s">
         <v>11</v>
       </c>
       <c r="B8" s="45" t="s">
@@ -3702,7 +3850,7 @@
       </c>
     </row>
     <row r="9" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="65"/>
+      <c r="A9" s="73"/>
       <c r="B9" s="48" t="s">
         <v>6</v>
       </c>
@@ -3720,7 +3868,7 @@
       </c>
     </row>
     <row r="10" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="65"/>
+      <c r="A10" s="73"/>
       <c r="B10" s="45" t="s">
         <v>7</v>
       </c>
@@ -3738,7 +3886,7 @@
       </c>
     </row>
     <row r="11" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="65"/>
+      <c r="A11" s="73"/>
       <c r="B11" s="48" t="s">
         <v>8</v>
       </c>
@@ -3754,7 +3902,7 @@
       </c>
     </row>
     <row r="12" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="65"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="45" t="s">
         <v>9</v>
       </c>
@@ -3772,7 +3920,7 @@
       </c>
     </row>
     <row r="13" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="74"/>
       <c r="B13" s="51" t="s">
         <v>10</v>
       </c>
@@ -3790,7 +3938,7 @@
       </c>
     </row>
     <row r="14" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="72" t="s">
         <v>15</v>
       </c>
       <c r="B14" s="45" t="s">
@@ -3810,7 +3958,7 @@
       </c>
     </row>
     <row r="15" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="65"/>
+      <c r="A15" s="73"/>
       <c r="B15" s="48" t="s">
         <v>6</v>
       </c>
@@ -3828,7 +3976,7 @@
       </c>
     </row>
     <row r="16" spans="1:22" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
+      <c r="A16" s="73"/>
       <c r="B16" s="45" t="s">
         <v>7</v>
       </c>
@@ -3846,7 +3994,7 @@
       </c>
     </row>
     <row r="17" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="73"/>
       <c r="B17" s="48" t="s">
         <v>8</v>
       </c>
@@ -3864,7 +4012,7 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65"/>
+      <c r="A18" s="73"/>
       <c r="B18" s="45" t="s">
         <v>9</v>
       </c>
@@ -3882,7 +4030,7 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="74"/>
       <c r="B19" s="51" t="s">
         <v>10</v>
       </c>
@@ -3900,7 +4048,7 @@
       </c>
     </row>
     <row r="20" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="72" t="s">
         <v>16</v>
       </c>
       <c r="B20" s="45" t="s">
@@ -3920,7 +4068,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="65"/>
+      <c r="A21" s="73"/>
       <c r="B21" s="48" t="s">
         <v>6</v>
       </c>
@@ -3938,7 +4086,7 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="65"/>
+      <c r="A22" s="73"/>
       <c r="B22" s="45" t="s">
         <v>7</v>
       </c>
@@ -3956,7 +4104,7 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="65"/>
+      <c r="A23" s="73"/>
       <c r="B23" s="48" t="s">
         <v>8</v>
       </c>
@@ -3974,7 +4122,7 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
+      <c r="A24" s="73"/>
       <c r="B24" s="45" t="s">
         <v>9</v>
       </c>
@@ -3992,7 +4140,7 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="74"/>
       <c r="B25" s="51" t="s">
         <v>10</v>
       </c>
@@ -4010,7 +4158,7 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="72" t="s">
         <v>19</v>
       </c>
       <c r="B26" s="48" t="s">
@@ -4030,7 +4178,7 @@
       </c>
     </row>
     <row r="27" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="65"/>
+      <c r="A27" s="73"/>
       <c r="B27" s="45" t="s">
         <v>6</v>
       </c>
@@ -4048,7 +4196,7 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="65"/>
+      <c r="A28" s="73"/>
       <c r="B28" s="48" t="s">
         <v>7</v>
       </c>
@@ -4066,7 +4214,7 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="65"/>
+      <c r="A29" s="73"/>
       <c r="B29" s="45" t="s">
         <v>8</v>
       </c>
@@ -4082,7 +4230,7 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="65"/>
+      <c r="A30" s="73"/>
       <c r="B30" s="48" t="s">
         <v>9</v>
       </c>
@@ -4100,7 +4248,7 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="66"/>
+      <c r="A31" s="74"/>
       <c r="B31" s="62" t="s">
         <v>10</v>
       </c>
@@ -4118,7 +4266,7 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="64" t="s">
+      <c r="A32" s="72" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="48" t="s">
@@ -4138,7 +4286,7 @@
       </c>
     </row>
     <row r="33" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="65"/>
+      <c r="A33" s="73"/>
       <c r="B33" s="45" t="s">
         <v>6</v>
       </c>
@@ -4156,7 +4304,7 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="65"/>
+      <c r="A34" s="73"/>
       <c r="B34" s="48" t="s">
         <v>7</v>
       </c>
@@ -4174,7 +4322,7 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="65"/>
+      <c r="A35" s="73"/>
       <c r="B35" s="45" t="s">
         <v>8</v>
       </c>
@@ -4192,7 +4340,7 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="65"/>
+      <c r="A36" s="73"/>
       <c r="B36" s="48" t="s">
         <v>9</v>
       </c>
@@ -4210,7 +4358,7 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
+      <c r="A37" s="74"/>
       <c r="B37" s="62" t="s">
         <v>10</v>
       </c>
@@ -4228,7 +4376,7 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="64" t="s">
+      <c r="A38" s="72" t="s">
         <v>58</v>
       </c>
       <c r="B38" s="48" t="s">
@@ -4248,7 +4396,7 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="65"/>
+      <c r="A39" s="73"/>
       <c r="B39" s="45" t="s">
         <v>6</v>
       </c>
@@ -4264,7 +4412,7 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="65"/>
+      <c r="A40" s="73"/>
       <c r="B40" s="48" t="s">
         <v>7</v>
       </c>
@@ -4282,7 +4430,7 @@
       </c>
     </row>
     <row r="41" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="65"/>
+      <c r="A41" s="73"/>
       <c r="B41" s="45" t="s">
         <v>8</v>
       </c>
@@ -4298,7 +4446,7 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="65"/>
+      <c r="A42" s="73"/>
       <c r="B42" s="48" t="s">
         <v>9</v>
       </c>
@@ -4316,7 +4464,7 @@
       </c>
     </row>
     <row r="43" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
+      <c r="A43" s="74"/>
       <c r="B43" s="62" t="s">
         <v>10</v>
       </c>
@@ -4334,7 +4482,7 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="64" t="s">
+      <c r="A44" s="72" t="s">
         <v>13</v>
       </c>
       <c r="B44" s="45" t="s">
@@ -4352,7 +4500,7 @@
       </c>
     </row>
     <row r="45" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="65"/>
+      <c r="A45" s="73"/>
       <c r="B45" s="48" t="s">
         <v>6</v>
       </c>
@@ -4368,7 +4516,7 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="65"/>
+      <c r="A46" s="73"/>
       <c r="B46" s="45" t="s">
         <v>7</v>
       </c>
@@ -4386,7 +4534,7 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="65"/>
+      <c r="A47" s="73"/>
       <c r="B47" s="48" t="s">
         <v>8</v>
       </c>
@@ -4402,7 +4550,7 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="65"/>
+      <c r="A48" s="73"/>
       <c r="B48" s="45" t="s">
         <v>9</v>
       </c>
@@ -4420,7 +4568,7 @@
       </c>
     </row>
     <row r="49" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="66"/>
+      <c r="A49" s="74"/>
       <c r="B49" s="51" t="s">
         <v>10</v>
       </c>
@@ -4438,7 +4586,7 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="64" t="s">
+      <c r="A50" s="72" t="s">
         <v>20</v>
       </c>
       <c r="B50" s="48" t="s">
@@ -4456,7 +4604,7 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="65"/>
+      <c r="A51" s="73"/>
       <c r="B51" s="45" t="s">
         <v>6</v>
       </c>
@@ -4472,7 +4620,7 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="65"/>
+      <c r="A52" s="73"/>
       <c r="B52" s="48" t="s">
         <v>7</v>
       </c>
@@ -4488,7 +4636,7 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="65"/>
+      <c r="A53" s="73"/>
       <c r="B53" s="45" t="s">
         <v>8</v>
       </c>
@@ -4504,7 +4652,7 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="65"/>
+      <c r="A54" s="73"/>
       <c r="B54" s="48" t="s">
         <v>9</v>
       </c>
@@ -4522,7 +4670,7 @@
       </c>
     </row>
     <row r="55" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="66"/>
+      <c r="A55" s="74"/>
       <c r="B55" s="62" t="s">
         <v>10</v>
       </c>
@@ -4540,7 +4688,7 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="64" t="s">
+      <c r="A56" s="72" t="s">
         <v>14</v>
       </c>
       <c r="B56" s="45" t="s">
@@ -4558,7 +4706,7 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="65"/>
+      <c r="A57" s="73"/>
       <c r="B57" s="48" t="s">
         <v>6</v>
       </c>
@@ -4574,7 +4722,7 @@
       </c>
     </row>
     <row r="58" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="65"/>
+      <c r="A58" s="73"/>
       <c r="B58" s="45" t="s">
         <v>7</v>
       </c>
@@ -4590,7 +4738,7 @@
       </c>
     </row>
     <row r="59" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="65"/>
+      <c r="A59" s="73"/>
       <c r="B59" s="48" t="s">
         <v>8</v>
       </c>
@@ -4606,7 +4754,7 @@
       </c>
     </row>
     <row r="60" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="65"/>
+      <c r="A60" s="73"/>
       <c r="B60" s="45" t="s">
         <v>9</v>
       </c>
@@ -4622,7 +4770,7 @@
       </c>
     </row>
     <row r="61" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="66"/>
+      <c r="A61" s="74"/>
       <c r="B61" s="51" t="s">
         <v>10</v>
       </c>
@@ -4640,7 +4788,7 @@
       </c>
     </row>
     <row r="62" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="64" t="s">
+      <c r="A62" s="72" t="s">
         <v>17</v>
       </c>
       <c r="B62" s="59" t="s">
@@ -4658,7 +4806,7 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="65"/>
+      <c r="A63" s="73"/>
       <c r="B63" s="45" t="s">
         <v>6</v>
       </c>
@@ -4674,7 +4822,7 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="65"/>
+      <c r="A64" s="73"/>
       <c r="B64" s="48" t="s">
         <v>7</v>
       </c>
@@ -4692,7 +4840,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="65"/>
+      <c r="A65" s="73"/>
       <c r="B65" s="45" t="s">
         <v>8</v>
       </c>
@@ -4708,7 +4856,7 @@
       </c>
     </row>
     <row r="66" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="65"/>
+      <c r="A66" s="73"/>
       <c r="B66" s="48" t="s">
         <v>9</v>
       </c>
@@ -4724,7 +4872,7 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="66"/>
+      <c r="A67" s="74"/>
       <c r="B67" s="62" t="s">
         <v>10</v>
       </c>
@@ -4740,7 +4888,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="64" t="s">
+      <c r="A68" s="72" t="s">
         <v>18</v>
       </c>
       <c r="B68" s="48" t="s">
@@ -4758,7 +4906,7 @@
       </c>
     </row>
     <row r="69" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="65"/>
+      <c r="A69" s="73"/>
       <c r="B69" s="45" t="s">
         <v>6</v>
       </c>
@@ -4774,7 +4922,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="65"/>
+      <c r="A70" s="73"/>
       <c r="B70" s="48" t="s">
         <v>7</v>
       </c>
@@ -4790,7 +4938,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="65"/>
+      <c r="A71" s="73"/>
       <c r="B71" s="45" t="s">
         <v>8</v>
       </c>
@@ -4806,7 +4954,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="65"/>
+      <c r="A72" s="73"/>
       <c r="B72" s="48" t="s">
         <v>9</v>
       </c>
@@ -4822,7 +4970,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="66"/>
+      <c r="A73" s="74"/>
       <c r="B73" s="62" t="s">
         <v>10</v>
       </c>
@@ -4840,7 +4988,7 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="64" t="s">
+      <c r="A74" s="72" t="s">
         <v>57</v>
       </c>
       <c r="B74" s="48" t="s">
@@ -4858,7 +5006,7 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="65"/>
+      <c r="A75" s="73"/>
       <c r="B75" s="45" t="s">
         <v>6</v>
       </c>
@@ -4874,7 +5022,7 @@
       </c>
     </row>
     <row r="76" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="65"/>
+      <c r="A76" s="73"/>
       <c r="B76" s="48" t="s">
         <v>7</v>
       </c>
@@ -4890,7 +5038,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="65"/>
+      <c r="A77" s="73"/>
       <c r="B77" s="45" t="s">
         <v>8</v>
       </c>
@@ -4906,7 +5054,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A78" s="65"/>
+      <c r="A78" s="73"/>
       <c r="B78" s="48" t="s">
         <v>9</v>
       </c>
@@ -4924,7 +5072,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A79" s="66"/>
+      <c r="A79" s="74"/>
       <c r="B79" s="62" t="s">
         <v>10</v>
       </c>
@@ -4942,7 +5090,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A80" s="64" t="s">
+      <c r="A80" s="72" t="s">
         <v>12</v>
       </c>
       <c r="B80" s="45" t="s">
@@ -4960,7 +5108,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="65"/>
+      <c r="A81" s="73"/>
       <c r="B81" s="48" t="s">
         <v>6</v>
       </c>
@@ -4976,7 +5124,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="65"/>
+      <c r="A82" s="73"/>
       <c r="B82" s="45" t="s">
         <v>7</v>
       </c>
@@ -4992,7 +5140,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="65"/>
+      <c r="A83" s="73"/>
       <c r="B83" s="48" t="s">
         <v>8</v>
       </c>
@@ -5008,7 +5156,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="65"/>
+      <c r="A84" s="73"/>
       <c r="B84" s="45" t="s">
         <v>9</v>
       </c>
@@ -5024,7 +5172,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A85" s="66"/>
+      <c r="A85" s="74"/>
       <c r="B85" s="51" t="s">
         <v>10</v>
       </c>
@@ -5087,36 +5235,36 @@
     <mergeCell ref="A32:A37"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A7">
-    <cfRule type="containsText" dxfId="45" priority="6" stopIfTrue="1" operator="containsText" text="LH">
+    <cfRule type="containsText" dxfId="56" priority="6" stopIfTrue="1" operator="containsText" text="LH">
       <formula>NOT(ISERROR(SEARCH("LH",A3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C2:C85">
-    <cfRule type="containsText" dxfId="44" priority="5" operator="containsText" text="LH">
+    <cfRule type="containsText" dxfId="55" priority="8" operator="containsText" text="HH">
+      <formula>NOT(ISERROR(SEARCH("HH",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="54" priority="10" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="53" priority="9" operator="containsText" text="&lt;100">
+      <formula>NOT(ISERROR(SEARCH("&lt;100",C2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="52" priority="5" operator="containsText" text="LH">
       <formula>NOT(ISERROR(SEARCH("LH",C2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="51" priority="7" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="8" operator="containsText" text="HH">
-      <formula>NOT(ISERROR(SEARCH("HH",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="9" operator="containsText" text="&lt;100">
-      <formula>NOT(ISERROR(SEARCH("&lt;100",C2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="40" priority="10" operator="containsText" text="T">
-      <formula>NOT(ISERROR(SEARCH("T",C2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D85">
-    <cfRule type="endsWith" dxfId="39" priority="1" operator="endsWith" text="*">
+    <cfRule type="endsWith" dxfId="50" priority="1" operator="endsWith" text="*">
       <formula>RIGHT(D2,LEN("*"))="*"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="38" priority="3" operator="endsWith" text="~">
+    <cfRule type="containsText" dxfId="49" priority="4" operator="containsText" text="P+">
+      <formula>NOT(ISERROR(SEARCH("P+",D2)))</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="48" priority="3" operator="endsWith" text="~">
       <formula>RIGHT(D2,LEN("~"))="~"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="37" priority="4" operator="containsText" text="P+">
-      <formula>NOT(ISERROR(SEARCH("P+",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:F85">
@@ -5130,7 +5278,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="35" priority="388" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="46" priority="388" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5140,6 +5288,7 @@
     <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000&amp;F&amp;R&amp;"Calibri,Regular"&amp;K000000&amp;D</oddHeader>
     <oddFooter>Page &amp;P of &amp;N</oddFooter>
   </headerFooter>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
@@ -5184,7 +5333,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3197C894-2AA6-D547-86AC-4C9C72092436}">
   <dimension ref="B1:G93"/>
   <sheetViews>
-    <sheetView topLeftCell="A41" zoomScale="180" zoomScaleNormal="180" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -6856,31 +7005,31 @@
     <sortCondition ref="G2:G85" customList="+,-,b"/>
   </sortState>
   <conditionalFormatting sqref="D2:D85">
-    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="LH">
+    <cfRule type="containsText" dxfId="44" priority="9" operator="containsText" text="&lt;100">
+      <formula>NOT(ISERROR(SEARCH("&lt;100",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="43" priority="10" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="42" priority="8" operator="containsText" text="HH">
+      <formula>NOT(ISERROR(SEARCH("HH",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="41" priority="5" operator="containsText" text="LH">
       <formula>NOT(ISERROR(SEARCH("LH",D2)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="40" priority="7" operator="equal">
       <formula>0</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="8" operator="containsText" text="HH">
-      <formula>NOT(ISERROR(SEARCH("HH",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="30" priority="9" operator="containsText" text="&lt;100">
-      <formula>NOT(ISERROR(SEARCH("&lt;100",D2)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="T">
-      <formula>NOT(ISERROR(SEARCH("T",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E85">
-    <cfRule type="endsWith" dxfId="28" priority="1" operator="endsWith" text="*">
+    <cfRule type="containsText" dxfId="39" priority="4" operator="containsText" text="P+">
+      <formula>NOT(ISERROR(SEARCH("P+",E2)))</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="38" priority="1" operator="endsWith" text="*">
       <formula>RIGHT(E2,LEN("*"))="*"</formula>
     </cfRule>
-    <cfRule type="endsWith" dxfId="27" priority="3" operator="endsWith" text="~">
+    <cfRule type="endsWith" dxfId="37" priority="3" operator="endsWith" text="~">
       <formula>RIGHT(E2,LEN("~"))="~"</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="4" operator="containsText" text="P+">
-      <formula>NOT(ISERROR(SEARCH("P+",E2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:G85">
@@ -6894,7 +7043,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6948,10 +7097,1777 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30AB5D69-D39A-4F42-9978-563297D57C07}">
+  <dimension ref="B1:G93"/>
+  <sheetViews>
+    <sheetView topLeftCell="A38" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="5" width="10.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:7" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="F2" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G2" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C7" s="29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>36</v>
+      </c>
+      <c r="F7" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="G7" s="42" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F8" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G8" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F9" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E10" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="11" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F11" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G11" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="14" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F14" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G14" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F15" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="F16" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G16" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F17" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G17" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F18" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G18" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C19" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D19" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G20" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E22" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G22" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G23" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F24" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C25" s="25" t="s">
+        <v>6</v>
+      </c>
+      <c r="D25" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="F25" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="G25" s="27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G26" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E27" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G27" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E28" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>42</v>
+      </c>
+      <c r="G29" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E31" s="79" t="s">
+        <v>36</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G31" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E32" s="40" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>36</v>
+      </c>
+      <c r="F33" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F34" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G34" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E35" s="41" t="s">
+        <v>38</v>
+      </c>
+      <c r="F35" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="G35" s="23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="36" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="37" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E37" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F37" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G37" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="38" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F39" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B40" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E40" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="41" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E41" s="33" t="s">
+        <v>38</v>
+      </c>
+      <c r="F41" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G41" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="42" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G42" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="C43" s="25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>23</v>
+      </c>
+      <c r="E43" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="F43" s="26" t="s">
+        <v>42</v>
+      </c>
+      <c r="G43" s="26" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C44" s="37" t="s">
+        <v>8</v>
+      </c>
+      <c r="D44" s="39" t="s">
+        <v>23</v>
+      </c>
+      <c r="E44" s="80" t="s">
+        <v>38</v>
+      </c>
+      <c r="F44" s="39" t="s">
+        <v>42</v>
+      </c>
+      <c r="G44" s="39" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="36" t="s">
+        <v>74</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E45" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F45" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G45" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B46" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E46" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F46" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G46" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="47" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E47" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F47" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="E48" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F48" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G48" s="6" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="49" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B49" s="36" t="s">
+        <v>76</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>38</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>42</v>
+      </c>
+      <c r="G49" s="28" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="50" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B50" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D50" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="51" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E51" s="6"/>
+      <c r="F51" s="24" t="s">
+        <v>43</v>
+      </c>
+      <c r="G51" s="24" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="52" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D52" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E52" s="5"/>
+      <c r="F52" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D53" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="5"/>
+      <c r="F53" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="54" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E54" s="5"/>
+      <c r="F54" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="55" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="56" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E56" s="5"/>
+      <c r="F56" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="57" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B57" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E57" s="5"/>
+      <c r="F57" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G57" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="58" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B58" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="6">
+        <v>0</v>
+      </c>
+      <c r="E58" s="6"/>
+      <c r="F58" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G58" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="59" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B59" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E59" s="5"/>
+      <c r="F59" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G59" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="60" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B60" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D60" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E60" s="6"/>
+      <c r="F60" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G60" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="61" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B61" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>9</v>
+      </c>
+      <c r="D61" s="28">
+        <v>0</v>
+      </c>
+      <c r="E61" s="5"/>
+      <c r="F61" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G61" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="62" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B62" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="C62" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G62" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="63" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B63" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E63" s="5"/>
+      <c r="F63" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G63" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="64" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B64" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="C64" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E64" s="6"/>
+      <c r="F64" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G64" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B65" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D65" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E65" s="5"/>
+      <c r="F65" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G65" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B66" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D66" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E66" s="6"/>
+      <c r="F66" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G66" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C67" s="29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="E67" s="28"/>
+      <c r="F67" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="G67" s="42" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B68" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E68" s="6"/>
+      <c r="F68" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="G68" s="24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B69" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D69" s="5">
+        <v>0</v>
+      </c>
+      <c r="E69" s="5"/>
+      <c r="F69" s="23" t="s">
+        <v>44</v>
+      </c>
+      <c r="G69" s="23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B70" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C70" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D70" s="38">
+        <v>0</v>
+      </c>
+      <c r="E70" s="38"/>
+      <c r="F70" s="43" t="s">
+        <v>44</v>
+      </c>
+      <c r="G70" s="38" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B71" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D71" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E71" s="5"/>
+      <c r="F71" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B72" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D72" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E72" s="5"/>
+      <c r="F72" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B73" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="C73" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="D73" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E73" s="26"/>
+      <c r="F73" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G73" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B74" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C74" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D74" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E74" s="6"/>
+      <c r="F74" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G74" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E75" s="5"/>
+      <c r="F75" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G75" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B76" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D76" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E76" s="6"/>
+      <c r="F76" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G76" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B77" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D77" s="5">
+        <v>0</v>
+      </c>
+      <c r="E77" s="5"/>
+      <c r="F77" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G77" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B78" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="C78" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G78" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B79" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="D79" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="E79" s="26"/>
+      <c r="F79" s="26" t="s">
+        <v>44</v>
+      </c>
+      <c r="G79" s="26" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D80" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="E80" s="5"/>
+      <c r="F80" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G80" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="81" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B81" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D81" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E81" s="6"/>
+      <c r="F81" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G81" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="82" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D82" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E82" s="5"/>
+      <c r="F82" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="G82" s="5" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="83" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B83" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C83" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D83" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E83" s="6"/>
+      <c r="F83" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G83" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="84" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B84" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C84" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E84" s="6"/>
+      <c r="F84" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="G84" s="6" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="85" spans="2:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B85" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="C85" s="29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D85" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="E85" s="28"/>
+      <c r="F85" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="G85" s="28" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="88" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B88" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="89" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B89" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="90" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B90" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="91" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B91" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="92" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B92" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="93" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B93" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:G85">
+    <sortCondition ref="E2:E85"/>
+  </sortState>
+  <conditionalFormatting sqref="D2:D85">
+    <cfRule type="containsText" dxfId="7" priority="4" operator="containsText" text="LH">
+      <formula>NOT(ISERROR(SEARCH("LH",D2)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="6" operator="containsText" text="HH">
+      <formula>NOT(ISERROR(SEARCH("HH",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="10" priority="7" operator="containsText" text="&lt;100">
+      <formula>NOT(ISERROR(SEARCH("&lt;100",D2)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E2:E85">
+    <cfRule type="endsWith" dxfId="4" priority="1" operator="endsWith" text="*">
+      <formula>RIGHT(E2,LEN("*"))="*"</formula>
+    </cfRule>
+    <cfRule type="endsWith" dxfId="3" priority="2" operator="endsWith" text="~">
+      <formula>RIGHT(E2,LEN("~"))="~"</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="P+">
+      <formula>NOT(ISERROR(SEARCH("P+",E2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:G85">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="11" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",F2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <headerFooter>
+    <oddHeader>&amp;L&amp;"Calibri,Regular"&amp;K000000&amp;F&amp;R&amp;"Calibri,Regular"&amp;K000000&amp;D</oddHeader>
+    <oddFooter>Page &amp;P of &amp;N</oddFooter>
+  </headerFooter>
+  <rowBreaks count="1" manualBreakCount="1">
+    <brk id="37" max="16383" man="1"/>
+  </rowBreaks>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="10" operator="containsText" id="{27E00B67-D116-5B43-9061-DCF7F6579C44}">
+            <xm:f>NOT(ISERROR(SEARCH("-",F2)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{ABE0AD4B-1931-EC4D-A306-7BED6AA73931}">
+            <xm:f>NOT(ISERROR(SEARCH("+",F2)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F2:G85</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B25E594E-1B71-8441-BE0D-247D4A871945}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -7028,7 +8944,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="69" t="s">
+      <c r="A10" s="64" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="17" t="s">
@@ -7037,7 +8953,7 @@
       <c r="C10" s="18"/>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="70" t="s">
+      <c r="A11" s="65" t="s">
         <v>38</v>
       </c>
       <c r="B11" s="19" t="s">
@@ -7046,7 +8962,7 @@
       <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:3" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="71" t="s">
+      <c r="A12" s="66" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="21" t="s">
@@ -7059,11 +8975,11 @@
       <c r="A14" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B14" s="72"/>
-      <c r="C14" s="73"/>
+      <c r="B14" s="77"/>
+      <c r="C14" s="78"/>
     </row>
     <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="67" t="s">
         <v>42</v>
       </c>
       <c r="B15" s="75" t="s">
@@ -7072,7 +8988,7 @@
       <c r="C15" s="76"/>
     </row>
     <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A16" s="77" t="s">
+      <c r="A16" s="68" t="s">
         <v>43</v>
       </c>
       <c r="B16" s="75" t="s">
@@ -7081,7 +8997,7 @@
       <c r="C16" s="76"/>
     </row>
     <row r="17" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="78" t="s">
+      <c r="A17" s="69" t="s">
         <v>44</v>
       </c>
       <c r="B17" s="21" t="s">
@@ -7094,11 +9010,11 @@
       <c r="A19" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="B19" s="72"/>
-      <c r="C19" s="73"/>
+      <c r="B19" s="77"/>
+      <c r="C19" s="78"/>
     </row>
     <row r="20" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A20" s="74" t="s">
+      <c r="A20" s="67" t="s">
         <v>42</v>
       </c>
       <c r="B20" s="75" t="s">
@@ -7107,7 +9023,7 @@
       <c r="C20" s="76"/>
     </row>
     <row r="21" spans="1:3" ht="17" x14ac:dyDescent="0.2">
-      <c r="A21" s="77" t="s">
+      <c r="A21" s="68" t="s">
         <v>43</v>
       </c>
       <c r="B21" s="75" t="s">
@@ -7116,7 +9032,7 @@
       <c r="C21" s="76"/>
     </row>
     <row r="22" spans="1:3" ht="18" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="78" t="s">
+      <c r="A22" s="69" t="s">
         <v>44</v>
       </c>
       <c r="B22" s="21" t="s">
@@ -7134,23 +9050,26 @@
     <mergeCell ref="B20:C20"/>
   </mergeCells>
   <conditionalFormatting sqref="A3:A7">
-    <cfRule type="cellIs" dxfId="22" priority="25" operator="equal">
-      <formula>0</formula>
+    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="T">
+      <formula>NOT(ISERROR(SEARCH("T",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="HH">
+    <cfRule type="containsText" dxfId="32" priority="28" operator="containsText" text="LH">
+      <formula>NOT(ISERROR(SEARCH("LH",A3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="27" operator="containsText" text="&lt;100">
+      <formula>NOT(ISERROR(SEARCH("&lt;100",A3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="26" operator="containsText" text="HH">
       <formula>NOT(ISERROR(SEARCH("HH",A3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="27" operator="containsText" text="&lt;100">
-      <formula>NOT(ISERROR(SEARCH("&lt;100",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="19" priority="28" operator="containsText" text="LH">
-      <formula>NOT(ISERROR(SEARCH("LH",A3)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="18" priority="29" operator="containsText" text="T">
-      <formula>NOT(ISERROR(SEARCH("T",A3)))</formula>
+    <cfRule type="cellIs" dxfId="29" priority="25" operator="equal">
+      <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A15">
+    <cfRule type="containsText" dxfId="27" priority="23" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",A15)))</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
@@ -7161,26 +9080,11 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="23" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",A15)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A20">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="19" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",A20)))</formula>
-    </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
+    <cfRule type="containsText" dxfId="25" priority="15" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",A16)))</formula>
+    </cfRule>
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
@@ -7190,39 +9094,6 @@
         <color rgb="FFFFEB84"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="15" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",A16)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A21">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="11" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",A21)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A22">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="b">
-      <formula>NOT(ISERROR(SEARCH("b",A22)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
@@ -7236,8 +9107,53 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="b">
+    <cfRule type="containsText" dxfId="22" priority="3" operator="containsText" text="b">
       <formula>NOT(ISERROR(SEARCH("b",A17)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A20">
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",A20)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="17">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A21">
+    <cfRule type="containsText" dxfId="16" priority="11" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",A21)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A22">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="b">
+      <formula>NOT(ISERROR(SEARCH("b",A22)))</formula>
+    </cfRule>
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -7246,6 +9162,20 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{9F6972C4-0D7F-554D-8555-41BB16D2B38B}">
+            <xm:f>NOT(ISERROR(SEARCH("+",A15)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
           <x14:cfRule type="containsText" priority="22" operator="containsText" id="{08E1CCC6-247F-304E-925A-A333D0E8F0E6}">
             <xm:f>NOT(ISERROR(SEARCH("-",A15)))</xm:f>
             <xm:f>"-"</xm:f>
@@ -7260,8 +9190,25 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="24" operator="containsText" id="{9F6972C4-0D7F-554D-8555-41BB16D2B38B}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A15)))</xm:f>
+          <xm:sqref>A15</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{5C403BB1-1BBF-4143-9995-05F3EC893B09}">
+            <xm:f>NOT(ISERROR(SEARCH("-",A16)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{AF9C4A07-EB81-8143-835D-E07CF16FB910}">
+            <xm:f>NOT(ISERROR(SEARCH("+",A16)))</xm:f>
             <xm:f>"+"</xm:f>
             <x14:dxf>
               <font>
@@ -7274,7 +9221,38 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A15</xm:sqref>
+          <xm:sqref>A16</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{F05A1241-8E90-BB4F-AD0E-97654444745C}">
+            <xm:f>NOT(ISERROR(SEARCH("-",A17)))</xm:f>
+            <xm:f>"-"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF006100"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFC6EFCE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{E19EFB69-5267-A142-9C46-59C38712D36C}">
+            <xm:f>NOT(ISERROR(SEARCH("+",A17)))</xm:f>
+            <xm:f>"+"</xm:f>
+            <x14:dxf>
+              <font>
+                <color rgb="FF9C0006"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor rgb="FFFFC7CE"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A17</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="18" operator="containsText" id="{A937F7D2-478E-1142-9D49-C39F188BA17D}">
@@ -7308,22 +9286,8 @@
           <xm:sqref>A20</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="14" operator="containsText" id="{5C403BB1-1BBF-4143-9995-05F3EC893B09}">
-            <xm:f>NOT(ISERROR(SEARCH("-",A16)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="16" operator="containsText" id="{AF9C4A07-EB81-8143-835D-E07CF16FB910}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A16)))</xm:f>
+          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{D2BB157C-BEA4-DD4D-A3A7-07B1B153AB06}">
+            <xm:f>NOT(ISERROR(SEARCH("+",A21)))</xm:f>
             <xm:f>"+"</xm:f>
             <x14:dxf>
               <font>
@@ -7336,9 +9300,6 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A16</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="10" operator="containsText" id="{80C3D04D-3808-574F-9A7B-EDBFEF5D28E3}">
             <xm:f>NOT(ISERROR(SEARCH("-",A21)))</xm:f>
             <xm:f>"-"</xm:f>
@@ -7353,8 +9314,11 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="12" operator="containsText" id="{D2BB157C-BEA4-DD4D-A3A7-07B1B153AB06}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A21)))</xm:f>
+          <xm:sqref>A21</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{E0A9DB55-BDAE-7643-8D48-ED04D75E11A3}">
+            <xm:f>NOT(ISERROR(SEARCH("+",A22)))</xm:f>
             <xm:f>"+"</xm:f>
             <x14:dxf>
               <font>
@@ -7367,9 +9331,6 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <xm:sqref>A21</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="containsText" priority="6" operator="containsText" id="{12E001BF-E2BC-1E4E-93A6-67BE18E18AFA}">
             <xm:f>NOT(ISERROR(SEARCH("-",A22)))</xm:f>
             <xm:f>"-"</xm:f>
@@ -7384,52 +9345,7 @@
               </fill>
             </x14:dxf>
           </x14:cfRule>
-          <x14:cfRule type="containsText" priority="8" operator="containsText" id="{E0A9DB55-BDAE-7643-8D48-ED04D75E11A3}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A22)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
           <xm:sqref>A22</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="containsText" priority="2" operator="containsText" id="{F05A1241-8E90-BB4F-AD0E-97654444745C}">
-            <xm:f>NOT(ISERROR(SEARCH("-",A17)))</xm:f>
-            <xm:f>"-"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF006100"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFC6EFCE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <x14:cfRule type="containsText" priority="4" operator="containsText" id="{E19EFB69-5267-A142-9C46-59C38712D36C}">
-            <xm:f>NOT(ISERROR(SEARCH("+",A17)))</xm:f>
-            <xm:f>"+"</xm:f>
-            <x14:dxf>
-              <font>
-                <color rgb="FF9C0006"/>
-              </font>
-              <fill>
-                <patternFill>
-                  <bgColor rgb="FFFFC7CE"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>A17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>